<commit_message>
update template header and title
</commit_message>
<xml_diff>
--- a/template/template_dnp.xlsx
+++ b/template/template_dnp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\laporan-kepegawaian\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DEC29B-2FA1-49A4-8E72-7A0472A8ABA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED78B42B-A59B-4998-B4CB-A61C65B3A8AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{31409149-ADB9-45E6-B40D-18E3E6D4E3DC}"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{31409149-ADB9-45E6-B40D-18E3E6D4E3DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -131,7 +131,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,9 +142,25 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -182,23 +198,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -516,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{934081F6-861B-4927-B820-7F825DC93BB1}">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -537,167 +555,172 @@
     <col min="16" max="16" width="24.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:16" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
+    <row r="2" spans="1:16" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3" t="s">
+      <c r="K4" s="5"/>
+      <c r="L4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3" t="s">
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="P4" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+    <row r="5" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
       <c r="F5" s="6"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3" t="s">
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3" t="s">
+      <c r="K5" s="5"/>
+      <c r="L5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+    <row r="6" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="2" t="s">
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="3"/>
-      <c r="M6" s="2" t="s">
+      <c r="L6" s="5"/>
+      <c r="M6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="N6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="3"/>
-      <c r="L7" s="2" t="s">
+      <c r="K7" s="5"/>
+      <c r="L7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="M7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="N7" s="3"/>
-      <c r="O7" s="2" t="s">
+      <c r="N7" s="5"/>
+      <c r="O7" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="P7" s="8" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:N4"/>
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="A4:B6"/>
     <mergeCell ref="C4:C6"/>
@@ -712,11 +735,6 @@
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:N5"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>